<commit_message>
Added an additional word and corrected some verse references.
</commit_message>
<xml_diff>
--- a/Crossword_Answers.xlsx
+++ b/Crossword_Answers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="23">
   <si>
     <t>A</t>
   </si>
@@ -511,7 +511,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +795,7 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L11" s="4" t="s">
@@ -811,6 +811,18 @@
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>

</xml_diff>